<commit_message>
Added AMD Model, fixed NVIDIA model.
</commit_message>
<xml_diff>
--- a/Nvidia DCF 10-26-22.xlsx
+++ b/Nvidia DCF 10-26-22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8415B9-43C2-C04E-AB1A-C03EFE029CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C87F4B-4820-0343-8D4B-BE4123AE998D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23560" yWindow="460" windowWidth="25700" windowHeight="26980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="460" windowWidth="25700" windowHeight="26980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -1081,10 +1081,10 @@
   <dimension ref="A1:AF112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="V56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AA7" sqref="AA7"/>
+      <selection pane="bottomRight" activeCell="Z67" sqref="Z67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8989,15 +8989,15 @@
       </c>
       <c r="Z99" s="45">
         <f>Y99*(1+Z100)</f>
-        <v>10408960000</v>
+        <v>10165000000</v>
       </c>
       <c r="AA99" s="45">
         <f>Z99*(1+AA100)</f>
-        <v>13323468800</v>
+        <v>12706250000</v>
       </c>
       <c r="AB99" s="45">
         <f>(AA99*(1+AB100))/(AD55-AB100)</f>
-        <v>156601565402.72476</v>
+        <v>149346890833.59219</v>
       </c>
       <c r="AC99" s="46" t="s">
         <v>124</v>
@@ -9068,7 +9068,7 @@
         <v>-0.16816519798915142</v>
       </c>
       <c r="Q100" s="17">
-        <f t="shared" ref="Q100:AB100" si="8">(Q99/P99)-1</f>
+        <f t="shared" ref="Q100:Y100" si="8">(Q99/P99)-1</f>
         <v>-9.5032791719915188E-2</v>
       </c>
       <c r="R100" s="17">
@@ -9104,10 +9104,10 @@
         <v>0.73242437153813378</v>
       </c>
       <c r="Z100" s="39">
-        <v>0.28000000000000003</v>
+        <v>0.25</v>
       </c>
       <c r="AA100" s="39">
-        <v>0.28000000000000003</v>
+        <v>0.25</v>
       </c>
       <c r="AB100" s="40">
         <v>2.5000000000000001E-2</v>
@@ -9148,15 +9148,15 @@
       <c r="Y101" s="13"/>
       <c r="Z101" s="1">
         <f>Z99/(1+$AD$55)^Z98</f>
-        <v>9358843978.4492149</v>
+        <v>9139496072.7043114</v>
       </c>
       <c r="AA101" s="1">
         <f>AA99/(1+$AD$55)^AA98</f>
-        <v>10770777251.962015</v>
+        <v>10271813632.928864</v>
       </c>
       <c r="AB101" s="1">
         <f>AB99/(1+$AD$55)^AB98</f>
-        <v>126597705415.97318</v>
+        <v>120732980171.17804</v>
       </c>
     </row>
     <row r="103" spans="1:32" x14ac:dyDescent="0.2">
@@ -9165,7 +9165,7 @@
       </c>
       <c r="Z103" s="47">
         <f>SUM(Z101:AB101)</f>
-        <v>146727326646.3844</v>
+        <v>140144289876.81122</v>
       </c>
     </row>
     <row r="104" spans="1:32" x14ac:dyDescent="0.2">
@@ -9192,7 +9192,7 @@
       </c>
       <c r="Z106" s="49">
         <f>Z103-Z104+Z105</f>
-        <v>156248326646.3844</v>
+        <v>149665289876.81122</v>
       </c>
     </row>
     <row r="107" spans="1:32" x14ac:dyDescent="0.2">
@@ -9209,7 +9209,7 @@
       </c>
       <c r="Z108" s="51">
         <f>Z106/Z107</f>
-        <v>62.750331986499759</v>
+        <v>60.106542119201293</v>
       </c>
     </row>
     <row r="109" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -9239,7 +9239,7 @@
       </c>
       <c r="Z112" s="56">
         <f>(Z108/Z109)-1</f>
-        <v>-0.51341243806994608</v>
+        <v>-0.53391329001860044</v>
       </c>
     </row>
   </sheetData>

</xml_diff>